<commit_message>
i426--python external environment issue fix
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/impl_01_mapar_engine.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/impl_01_mapar_engine.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{F6466A3E-E8D6-4C17-8754-AC34666D29F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{19FD41B7-6767-4BD4-B7B1-CC394A76C821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -1050,13 +1050,13 @@
     <t>06_PAR_CMD_Command/151_dh</t>
   </si>
   <si>
-    <t>radiant=sd_ng3_2p.18</t>
-  </si>
-  <si>
     <t>cmd = --check-conf=impl.conf --post-process=syn_t.py</t>
   </si>
   <si>
     <t>cmd = --check-conf=impl.conf --run-export-bitstream</t>
+  </si>
+  <si>
+    <t>radiant=ng2022</t>
   </si>
   <si>
     <t>impl_01_mapar_engine_v2.01</t>
@@ -5000,7 +5000,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{269D2C2A-931E-45DB-A665-801146CA6E48}" diskRevisions="1" revisionId="303" version="24">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BF04477F-E450-46DA-9380-B089DC7A40AD}" diskRevisions="1" revisionId="304" version="25">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5185,7 +5185,15 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
-  <header guid="{269D2C2A-931E-45DB-A665-801146CA6E48}" dateTime="2022-07-08T16:31:17" maxSheetId="5" userName="Jason Wang" r:id="rId24" minRId="303">
+  <header guid="{157B790F-5B69-4EC0-98B8-87F5A8B8B29D}" dateTime="2022-08-17T09:45:21" maxSheetId="5" userName="Jason Wang" r:id="rId24" minRId="303">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BF04477F-E450-46DA-9380-B089DC7A40AD}" dateTime="2022-08-17T09:57:10" maxSheetId="5" userName="Jason Wang" r:id="rId25" minRId="304">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -7865,6 +7873,23 @@
 <file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="303" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=sd_ng3_2p.18</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2022</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="304" sId="1">
     <oc r="B3" t="inlineStr">
       <is>
         <t>impl_01_mapar_engine_v2.00</t>
@@ -8709,9 +8734,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
@@ -8773,7 +8800,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -8838,36 +8865,36 @@
       <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="2" customWidth="1"/>
     <col min="8" max="8" width="37" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="13" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" style="2" customWidth="1"/>
     <col min="21" max="21" width="11" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="2" customWidth="1"/>
     <col min="23" max="28" width="9" style="2"/>
-    <col min="29" max="29" width="10.140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="10.109375" style="2" customWidth="1"/>
     <col min="30" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:30" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A1" s="67" t="s">
         <v>15</v>
       </c>
@@ -8903,7 +8930,7 @@
       <c r="AC1" s="70"/>
       <c r="AD1" s="70"/>
     </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:30" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -8995,7 +9022,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" thickTop="1">
+    <row r="3" spans="1:30" ht="15" thickTop="1">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -9006,7 +9033,7 @@
         <v>306</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -9020,7 +9047,7 @@
         <v>307</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -9034,7 +9061,7 @@
         <v>303</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -9048,7 +9075,7 @@
         <v>304</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -9062,7 +9089,7 @@
         <v>305</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -9076,7 +9103,7 @@
         <v>308</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -9090,7 +9117,7 @@
         <v>309</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -9104,7 +9131,7 @@
         <v>310</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -9118,7 +9145,7 @@
         <v>312</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -9132,7 +9159,7 @@
         <v>313</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -9146,7 +9173,7 @@
         <v>314</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -9160,7 +9187,7 @@
         <v>315</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -9174,7 +9201,7 @@
         <v>316</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -9319,7 +9346,7 @@
         <v>319</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -9333,7 +9360,7 @@
         <v>320</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -9347,7 +9374,7 @@
         <v>321</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -9361,7 +9388,7 @@
         <v>322</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -9375,7 +9402,7 @@
         <v>323</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -9389,7 +9416,7 @@
         <v>324</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -9403,7 +9430,7 @@
         <v>325</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9415,35 +9442,35 @@
       <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2" xr:uid="{E33BA2B8-63BD-40A2-B719-00B2009D9951}"/>
+      <autoFilter ref="A2:AD2" xr:uid="{D841A358-E5AD-44AB-85C7-4276A4896879}"/>
     </customSheetView>
     <customSheetView guid="{935BDBD9-B387-4985-B478-6F8B21CA0B09}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:AD2" xr:uid="{FEBA112C-B54C-43DD-8FB9-4F0B42F1D42F}"/>
+      <autoFilter ref="A2:AD2" xr:uid="{A4C59B05-55B6-4C6B-AAE9-A6BDF06ECDA8}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2" xr:uid="{7F9FEC7E-735D-45D8-80AA-D346CB15336C}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{8BE20075-02B1-46FA-916A-E011DF396F51}"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:Y2" xr:uid="{103F00C0-770B-4FEA-85FB-212C16D64B20}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{4F7FABC4-6E61-4742-83A2-ACD5EF7DCE59}"/>
     </customSheetView>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-      <autoFilter ref="A2:AD2" xr:uid="{EC3DD8A9-FD29-4D41-9A11-A9CA47927F77}"/>
+      <autoFilter ref="A2:AD2" xr:uid="{F041957E-A77B-4626-9ED4-C42AFA113BFC}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -9526,18 +9553,18 @@
       <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="19" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="32" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -9560,7 +9587,7 @@
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="108" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="109" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="110" spans="1:14" ht="15.75" thickBot="1">
+    <row r="110" spans="1:14" ht="15" thickBot="1">
       <c r="A110" s="6" t="s">
         <v>81</v>
       </c>
@@ -9568,7 +9595,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15.75" thickBot="1">
+    <row r="111" spans="1:14" ht="15" thickBot="1">
       <c r="A111" s="9" t="s">
         <v>83</v>
       </c>
@@ -10396,7 +10423,7 @@
       <c r="M141" s="18"/>
       <c r="N141" s="19"/>
     </row>
-    <row r="142" spans="1:14" ht="15.75" thickBot="1">
+    <row r="142" spans="1:14" ht="15" thickBot="1">
       <c r="A142" s="20" t="s">
         <v>122</v>
       </c>
@@ -10420,7 +10447,7 @@
       <c r="M142" s="21"/>
       <c r="N142" s="22"/>
     </row>
-    <row r="145" spans="1:8" ht="15.75" thickBot="1">
+    <row r="145" spans="1:8" ht="15" thickBot="1">
       <c r="A145" s="6" t="s">
         <v>123</v>
       </c>
@@ -11038,7 +11065,7 @@
       </c>
       <c r="H172" s="16"/>
     </row>
-    <row r="173" spans="1:8" ht="90">
+    <row r="173" spans="1:8" ht="86.4">
       <c r="A173" s="26">
         <v>27</v>
       </c>
@@ -11132,7 +11159,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="15.75" thickBot="1">
+    <row r="177" spans="1:8" ht="15" thickBot="1">
       <c r="A177" s="31">
         <v>31</v>
       </c>
@@ -11288,7 +11315,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="15.75" thickBot="1">
+    <row r="184" spans="1:8" ht="15" thickBot="1">
       <c r="A184" s="35">
         <v>38</v>
       </c>
@@ -11328,7 +11355,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15.75" thickBot="1">
+    <row r="197" spans="1:7" ht="15" thickBot="1">
       <c r="A197" s="6" t="s">
         <v>207</v>
       </c>
@@ -11602,7 +11629,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="15.75" thickBot="1">
+    <row r="214" spans="1:7" ht="15" thickBot="1">
       <c r="A214" s="96"/>
       <c r="B214" s="97"/>
       <c r="C214" s="97" t="s">
@@ -11636,7 +11663,7 @@
       <c r="D217" s="37"/>
       <c r="E217" s="37"/>
     </row>
-    <row r="218" spans="1:7" ht="15.75" thickBot="1">
+    <row r="218" spans="1:7" ht="15" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>231</v>
       </c>
@@ -11644,7 +11671,7 @@
       <c r="D218" s="37"/>
       <c r="E218" s="37"/>
     </row>
-    <row r="219" spans="1:7" ht="15.75" thickBot="1">
+    <row r="219" spans="1:7" ht="15" thickBot="1">
       <c r="A219" s="45" t="s">
         <v>232</v>
       </c>
@@ -11732,12 +11759,12 @@
     <row r="224" spans="1:7">
       <c r="C224" s="51"/>
     </row>
-    <row r="226" spans="1:7" ht="15.75" thickBot="1">
+    <row r="226" spans="1:7" ht="15" thickBot="1">
       <c r="A226" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="15.75" thickBot="1">
+    <row r="227" spans="1:7" ht="15" thickBot="1">
       <c r="A227" s="9" t="s">
         <v>243</v>
       </c>
@@ -11977,7 +12004,7 @@
       <c r="F240" s="64"/>
       <c r="G240" s="43"/>
     </row>
-    <row r="241" spans="1:7" ht="15.75" thickBot="1">
+    <row r="241" spans="1:7" ht="15" thickBot="1">
       <c r="A241" s="65">
         <v>44118</v>
       </c>
@@ -12078,7 +12105,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>